<commit_message>
Correct sed_beh_sitting and HBA1C
</commit_message>
<xml_diff>
--- a/data_processing_elements-SHS.xlsx
+++ b/data_processing_elements-SHS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ABA3054-D2FE-4FAB-B52F-DDE837B8FE92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB1E88D9-8DD6-43DF-9AAC-D0C2BA70E5C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
@@ -1476,9 +1476,6 @@
 ELSE ~ NA_integer_)</t>
   </si>
   <si>
-    <t>(HBA1C*10.93) - 23.5</t>
-  </si>
-  <si>
     <t>round(calculated_LDL, 2)</t>
   </si>
   <si>
@@ -1493,40 +1490,6 @@
 rowSums(mutate(., temp_l2min = l2min/60) %&gt;% select(temp_l2min, l2hr), na.rm = TRUE) &lt;= 1 ~ 1L;
 rowSums(mutate(., temp_l2min = l2min/60) %&gt;% select(temp_l2min, l2hr), na.rm = TRUE) &gt; 1 &amp; rowSums(mutate(., temp_l2min = l2min/60) %&gt;% select(temp_l2min, l2hr), na.rm = TRUE) &lt;= 3 ~ 2L;
 rowSums(mutate(., temp_l2min = l2min/60) %&gt;% select(temp_l2min, l2hr), na.rm = TRUE) &gt; 3 ~ 3L;
-ELSE ~ NA_integer_)</t>
-  </si>
-  <si>
-    <t>rowSums(mutate(.,
-temp_l10min = l10min/60,
-temp_l12min = l12min/60) %&gt;%
-select(temp_l10min, l10hr, temp_l12min, l12hr), na.rm = TRUE)</t>
-  </si>
-  <si>
-    <t>case_when(
-rowSums(mutate(.,
-temp_l10min = l10min/60,
-temp_l12min = l12min/60) %&gt;%
-select(temp_l10min, l10hr, temp_l12min, l12hr), na.rm = TRUE) == 0 ~ 0L;
-rowSums(mutate(.,
-temp_l10min = l10min/60,
-temp_l12min = l12min/60) %&gt;%
-select(temp_l10min, l10hr, temp_l12min, l12hr), na.rm = TRUE) &lt; 1 ~ 1L;
-rowSums(mutate(.,
-temp_l10min = l10min/60,
-temp_l12min = l12min/60) %&gt;%
-select(temp_l10min, l10hr, temp_l12min, l12hr), na.rm = TRUE) &lt; 3 ~ 2L;
-rowSums(mutate(.,
-temp_l10min = l10min/60,
-temp_l12min = l12min/60) %&gt;%
-select(temp_l10min, l10hr, temp_l12min, l12hr), na.rm = TRUE) &lt; 5 ~ 3L;
-rowSums(mutate(.,
-temp_l10min = l10min/60,
-temp_l12min = l12min/60) %&gt;%
-select(temp_l10min, l10hr, temp_l12min, l12hr), na.rm = TRUE) &lt; 7 ~ 4L;
-rowSums(mutate(.,
-temp_l10min = l10min/60,
-temp_l12min = l12min/60) %&gt;%
-select(temp_l10min, l10hr, temp_l12min, l12hr), na.rm = TRUE) &gt;= 7 ~ 5L;
 ELSE ~ NA_integer_)</t>
   </si>
   <si>
@@ -1883,12 +1846,49 @@
 rowSums(mutate(., temp_l1min = l1min/60, temp_l2min = l2min/60) %&gt;% select(temp_l1min, temp_l2min, l1hr, l2hr), na.rm = TRUE) &gt; 3 ~ 3L;
 ELSE ~ NA_integer_)</t>
   </si>
+  <si>
+    <t>ifelse(!is.na(HBA1C),(HBA1C*10.93) - 23.5,NA)</t>
+  </si>
+  <si>
+    <t>rowSums(mutate(.,
+temp_l10min = ifelse(!is.na(l10min),l10min/60,NA),
+temp_l12min = ifelse(!is.na(l12min),l12min/60,NA)) %&gt;%
+select(temp_l10min, l10hr, temp_l12min, l12hr), na.rm = TRUE)</t>
+  </si>
+  <si>
+    <t>case_when(
+rowSums(mutate(.,
+temp_l10min = ifelse(!is.na(l10min),l10min/60,NA),
+temp_l12min = ifelse(!is.na(l12min),l12min/60,NA)) %&gt;%
+select(temp_l10min, l10hr, temp_l12min, l12hr), na.rm = TRUE) == 0 ~ 0L;
+rowSums(mutate(.,
+temp_l10min = ifelse(!is.na(l10min),l10min/60,NA),
+temp_l12min = ifelse(!is.na(l12min),l12min/60,NA)) %&gt;%
+select(temp_l10min, l10hr, temp_l12min, l12hr), na.rm = TRUE) &lt; 1 ~ 1L;
+rowSums(mutate(.,
+temp_l10min = ifelse(!is.na(l10min),l10min/60,NA),
+temp_l12min = ifelse(!is.na(l12min),l12min/60,NA)) %&gt;%
+select(temp_l10min, l10hr, temp_l12min, l12hr), na.rm = TRUE) &lt; 3 ~ 2L;
+rowSums(mutate(.,
+temp_l10min = ifelse(!is.na(l10min),l10min/60,NA),
+temp_l12min = ifelse(!is.na(l12min),l12min/60,NA)) %&gt;%
+select(temp_l10min, l10hr, temp_l12min, l12hr), na.rm = TRUE) &lt; 5 ~ 3L;
+rowSums(mutate(.,
+temp_l10min = ifelse(!is.na(l10min),l10min/60,NA),
+temp_l12min = ifelse(!is.na(l12min),l12min/60,NA)) %&gt;%
+select(temp_l10min, l10hr, temp_l12min, l12hr), na.rm = TRUE) &lt; 7 ~ 4L;
+rowSums(mutate(.,
+temp_l10min = ifelse(!is.na(l10min),l10min/60,NA),
+temp_l12min = ifelse(!is.na(l12min),l12min/60,NA)) %&gt;%
+select(temp_l10min, l10hr, temp_l12min, l12hr), na.rm = TRUE) &gt;= 7 ~ 5L;
+ELSE ~ NA_integer_)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1919,6 +1919,12 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1967,7 +1973,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2011,6 +2017,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2353,10 +2360,10 @@
   <dimension ref="A1:AD84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="S66" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="S72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W70" sqref="W70"/>
+      <selection pane="bottomRight" activeCell="X77" sqref="X77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="54.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2412,19 +2419,19 @@
         <v>10</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="M1" s="9" t="s">
         <v>11</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="Q1" s="4" t="s">
         <v>12</v>
@@ -2448,25 +2455,25 @@
         <v>18</v>
       </c>
       <c r="X1" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="Y1" t="s">
         <v>19</v>
       </c>
       <c r="Z1" t="s">
+        <v>489</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>490</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>491</v>
+      </c>
+      <c r="AC1" t="s">
         <v>492</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AD1" t="s">
         <v>493</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>494</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>495</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
@@ -2492,7 +2499,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="11"/>
       <c r="J2" s="1" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>296</v>
@@ -2515,7 +2522,7 @@
         <v>26</v>
       </c>
       <c r="W2" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="3" spans="1:30" ht="75" x14ac:dyDescent="0.25">
@@ -2543,7 +2550,7 @@
       </c>
       <c r="I3" s="11"/>
       <c r="J3" s="1" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>313</v>
@@ -2568,10 +2575,10 @@
         <v>32</v>
       </c>
       <c r="W3" t="s">
+        <v>439</v>
+      </c>
+      <c r="X3" t="s">
         <v>442</v>
-      </c>
-      <c r="X3" t="s">
-        <v>445</v>
       </c>
       <c r="Y3" s="14" t="s">
         <v>314</v>
@@ -2614,7 +2621,7 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="Q4" s="6" t="s">
         <v>317</v>
@@ -2670,7 +2677,7 @@
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>23</v>
@@ -2730,7 +2737,7 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="Q6" s="6" t="s">
         <v>323</v>
@@ -2750,7 +2757,7 @@
         <v>324</v>
       </c>
       <c r="X6" s="14" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="Y6" t="s">
         <v>288</v>
@@ -2793,7 +2800,7 @@
       <c r="N7" s="1"/>
       <c r="O7" s="6"/>
       <c r="P7" s="1" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="Q7" s="1" t="s">
         <v>327</v>
@@ -2815,7 +2822,7 @@
         <v>3</v>
       </c>
       <c r="X7" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="Y7" t="s">
         <v>329</v>
@@ -2858,7 +2865,7 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="Q8" s="6" t="s">
         <v>332</v>
@@ -2962,7 +2969,7 @@
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="Q10" s="6" t="s">
         <v>335</v>
@@ -2982,10 +2989,10 @@
         <v>61</v>
       </c>
       <c r="X10" s="14" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="Z10" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="11" spans="1:30" ht="180" x14ac:dyDescent="0.25">
@@ -3023,7 +3030,7 @@
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="Q11" s="6" t="s">
         <v>338</v>
@@ -3043,7 +3050,7 @@
         <v>339</v>
       </c>
       <c r="Z11" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="12" spans="1:30" ht="128.25" x14ac:dyDescent="0.25">
@@ -3083,7 +3090,7 @@
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="Q12" s="6" t="s">
         <v>332</v>
@@ -3103,7 +3110,7 @@
         <v>340</v>
       </c>
       <c r="Z12" s="14" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="13" spans="1:30" ht="85.5" x14ac:dyDescent="0.25">
@@ -3143,7 +3150,7 @@
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="Q13" s="6" t="s">
         <v>343</v>
@@ -3200,7 +3207,7 @@
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="Q14" s="6" t="s">
         <v>343</v>
@@ -3273,7 +3280,7 @@
         <v>2</v>
       </c>
       <c r="X15" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="Y15" t="s">
         <v>346</v>
@@ -3727,7 +3734,7 @@
         <v>61</v>
       </c>
       <c r="X23" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="Y23" t="s">
         <v>358</v>
@@ -3780,7 +3787,7 @@
         <v>61</v>
       </c>
       <c r="X24" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="Y24" t="s">
         <v>358</v>
@@ -4052,7 +4059,7 @@
         <v>426</v>
       </c>
       <c r="X29" s="14" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="Y29" t="s">
         <v>367</v>
@@ -4160,11 +4167,11 @@
       <c r="V31" t="s">
         <v>32</v>
       </c>
-      <c r="W31" t="s">
-        <v>427</v>
+      <c r="W31" s="17" t="s">
+        <v>495</v>
       </c>
       <c r="X31" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="Y31" t="s">
         <v>292</v>
@@ -4225,7 +4232,7 @@
         <v>45</v>
       </c>
       <c r="X32" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.25">
@@ -4283,7 +4290,7 @@
         <v>45</v>
       </c>
       <c r="X33" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.25">
@@ -4341,7 +4348,7 @@
         <v>45</v>
       </c>
       <c r="X34" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.25">
@@ -4380,7 +4387,7 @@
       </c>
       <c r="N35" s="1"/>
       <c r="O35" s="1" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
@@ -4400,7 +4407,7 @@
         <v>32</v>
       </c>
       <c r="W35" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.25">
@@ -4455,10 +4462,10 @@
         <v>32</v>
       </c>
       <c r="W36" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="X36" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.25">
@@ -4546,7 +4553,7 @@
       </c>
       <c r="N38" s="1"/>
       <c r="O38" s="1" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="P38" s="1" t="s">
         <v>44</v>
@@ -4569,7 +4576,7 @@
         <v>61</v>
       </c>
       <c r="X38" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="Y38" t="s">
         <v>302</v>
@@ -4660,7 +4667,7 @@
       </c>
       <c r="N40" s="1"/>
       <c r="O40" s="1" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="P40" s="1" t="s">
         <v>44</v>
@@ -4771,7 +4778,7 @@
       </c>
       <c r="N42" s="1"/>
       <c r="O42" s="1" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="P42" s="1" t="s">
         <v>44</v>
@@ -4794,7 +4801,7 @@
         <v>45</v>
       </c>
       <c r="X42" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="Y42" t="s">
         <v>377</v>
@@ -4852,10 +4859,10 @@
         <v>32</v>
       </c>
       <c r="W43" s="14" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="X43" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="Y43" s="14" t="s">
         <v>385</v>
@@ -4883,7 +4890,7 @@
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="15" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>386</v>
@@ -4898,7 +4905,7 @@
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
       <c r="P44" s="1" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="Q44" s="6" t="s">
         <v>389</v>
@@ -4999,7 +5006,7 @@
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="15" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="J46" s="6" t="s">
         <v>391</v>
@@ -5138,7 +5145,7 @@
         <v>61</v>
       </c>
       <c r="X48" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="Y48" t="s">
         <v>402</v>
@@ -5192,7 +5199,7 @@
         <v>61</v>
       </c>
       <c r="X49" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="Y49" t="s">
         <v>198</v>
@@ -5281,7 +5288,7 @@
       <c r="O51" s="1"/>
       <c r="P51" s="1"/>
       <c r="Q51" s="1" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="R51" s="1"/>
       <c r="S51" s="1"/>
@@ -5399,7 +5406,7 @@
         <v>61</v>
       </c>
       <c r="X53" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="Y53" t="s">
         <v>403</v>
@@ -5490,13 +5497,13 @@
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
       <c r="M55" s="11" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="N55" s="1"/>
       <c r="O55" s="1"/>
       <c r="P55" s="1"/>
       <c r="Q55" s="6" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="R55" s="1"/>
       <c r="S55" s="1"/>
@@ -5510,7 +5517,7 @@
         <v>38</v>
       </c>
       <c r="W55" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="Y55" t="s">
         <v>198</v>
@@ -5546,13 +5553,13 @@
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
       <c r="M56" s="11" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="N56" s="1"/>
       <c r="O56" s="1"/>
       <c r="P56" s="1"/>
       <c r="Q56" s="6" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="R56" s="1"/>
       <c r="S56" s="1"/>
@@ -5566,7 +5573,7 @@
         <v>38</v>
       </c>
       <c r="W56" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="Y56" t="s">
         <v>198</v>
@@ -5602,13 +5609,13 @@
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
       <c r="M57" s="11" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="N57" s="1"/>
       <c r="O57" s="1"/>
       <c r="P57" s="1"/>
       <c r="Q57" s="6" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="R57" s="1"/>
       <c r="S57" s="1"/>
@@ -5622,7 +5629,7 @@
         <v>38</v>
       </c>
       <c r="W57" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="Y57" t="s">
         <v>198</v>
@@ -6104,7 +6111,7 @@
         <v>61</v>
       </c>
       <c r="X67" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="Y67" t="s">
         <v>198</v>
@@ -6159,7 +6166,7 @@
         <v>61</v>
       </c>
       <c r="X68" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="Y68" t="s">
         <v>198</v>
@@ -6214,7 +6221,7 @@
         <v>61</v>
       </c>
       <c r="X69" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="Y69" t="s">
         <v>198</v>
@@ -6266,10 +6273,10 @@
         <v>205</v>
       </c>
       <c r="W70" s="14" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="X70" s="14" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="Y70" t="s">
         <v>198</v>
@@ -6321,7 +6328,7 @@
         <v>205</v>
       </c>
       <c r="W71" s="14" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="Y71" t="s">
         <v>198</v>
@@ -6373,7 +6380,7 @@
         <v>205</v>
       </c>
       <c r="W72" s="14" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="Y72" t="s">
         <v>198</v>
@@ -6572,7 +6579,7 @@
         <v>32</v>
       </c>
       <c r="W76" s="14" t="s">
-        <v>431</v>
+        <v>496</v>
       </c>
       <c r="Y76" t="s">
         <v>408</v>
@@ -6622,10 +6629,10 @@
         <v>205</v>
       </c>
       <c r="W77" s="14" t="s">
-        <v>432</v>
+        <v>497</v>
       </c>
       <c r="X77" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="Y77" t="s">
         <v>408</v>
@@ -6665,7 +6672,7 @@
       <c r="O78" s="1"/>
       <c r="P78" s="1"/>
       <c r="Q78" s="1" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="R78" s="1"/>
       <c r="S78" s="6"/>
@@ -6679,7 +6686,7 @@
         <v>205</v>
       </c>
       <c r="W78" s="14" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="Y78" t="s">
         <v>198</v>
@@ -6765,7 +6772,7 @@
         <v>189</v>
       </c>
       <c r="J80" s="6" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="K80" s="1"/>
       <c r="L80" s="1"/>
@@ -6776,7 +6783,7 @@
       <c r="Q80" s="1"/>
       <c r="R80" s="1"/>
       <c r="S80" s="6" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="T80" s="7" t="s">
         <v>24</v>
@@ -6788,7 +6795,7 @@
         <v>205</v>
       </c>
       <c r="W80" s="14" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="Y80" t="s">
         <v>198</v>
@@ -6824,13 +6831,13 @@
       <c r="K81" s="1"/>
       <c r="L81" s="1"/>
       <c r="M81" s="15" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="N81" s="1"/>
       <c r="O81" s="1"/>
       <c r="P81" s="1"/>
       <c r="Q81" s="1" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="R81" s="1"/>
       <c r="S81" s="6"/>
@@ -6844,7 +6851,7 @@
         <v>205</v>
       </c>
       <c r="W81" s="14" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="82" spans="1:25" ht="409.5" x14ac:dyDescent="0.25">
@@ -6872,7 +6879,7 @@
         <v>189</v>
       </c>
       <c r="J82" s="6" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="K82" s="1"/>
       <c r="L82" s="1"/>
@@ -6883,7 +6890,7 @@
       <c r="Q82" s="1"/>
       <c r="R82" s="1"/>
       <c r="S82" s="6" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="T82" s="7" t="s">
         <v>24</v>
@@ -6895,7 +6902,7 @@
         <v>205</v>
       </c>
       <c r="W82" s="14" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="Y82" t="s">
         <v>198</v>

</xml_diff>

<commit_message>
try to round the values for sed_beh_total_sitting
</commit_message>
<xml_diff>
--- a/data_processing_elements-SHS.xlsx
+++ b/data_processing_elements-SHS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB1E88D9-8DD6-43DF-9AAC-D0C2BA70E5C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9E582A-F6EE-40D2-A862-DDA98A18F59B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
@@ -1850,12 +1850,6 @@
     <t>ifelse(!is.na(HBA1C),(HBA1C*10.93) - 23.5,NA)</t>
   </si>
   <si>
-    <t>rowSums(mutate(.,
-temp_l10min = ifelse(!is.na(l10min),l10min/60,NA),
-temp_l12min = ifelse(!is.na(l12min),l12min/60,NA)) %&gt;%
-select(temp_l10min, l10hr, temp_l12min, l12hr), na.rm = TRUE)</t>
-  </si>
-  <si>
     <t>case_when(
 rowSums(mutate(.,
 temp_l10min = ifelse(!is.na(l10min),l10min/60,NA),
@@ -1882,6 +1876,12 @@
 temp_l12min = ifelse(!is.na(l12min),l12min/60,NA)) %&gt;%
 select(temp_l10min, l10hr, temp_l12min, l12hr), na.rm = TRUE) &gt;= 7 ~ 5L;
 ELSE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>round(rowSums(mutate(.,
+temp_l10min = ifelse(!is.na(l10min),l10min/60,NA),
+temp_l12min = ifelse(!is.na(l12min),l12min/60,NA)) %&gt;%
+select(temp_l10min, l10hr, temp_l12min, l12hr), na.rm = TRUE))</t>
   </si>
 </sst>
 </file>
@@ -2360,10 +2360,10 @@
   <dimension ref="A1:AD84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="S72" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="S73" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X77" sqref="X77"/>
+      <selection pane="bottomRight" activeCell="W77" sqref="W77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="54.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2382,6 +2382,7 @@
     <col min="13" max="13" width="60.7109375" style="13" customWidth="1"/>
     <col min="14" max="14" width="21.7109375" style="12" bestFit="1" customWidth="1"/>
     <col min="15" max="21" width="54.85546875" style="12"/>
+    <col min="23" max="23" width="74" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.25">
@@ -6533,7 +6534,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="76" spans="1:25" ht="75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:25" ht="60" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -6579,13 +6580,13 @@
         <v>32</v>
       </c>
       <c r="W76" s="14" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="Y76" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="77" spans="1:25" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:25" ht="390" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -6629,7 +6630,7 @@
         <v>205</v>
       </c>
       <c r="W77" s="14" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="X77" t="s">
         <v>480</v>

</xml_diff>

<commit_message>
correct hear rate, systo diasto bp, alcohol
</commit_message>
<xml_diff>
--- a/data_processing_elements-SHS.xlsx
+++ b/data_processing_elements-SHS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9E582A-F6EE-40D2-A862-DDA98A18F59B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D38B06AB-1D90-4985-92B5-232B53A04D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
@@ -1460,15 +1460,6 @@
   </si>
   <si>
     <t>round(rowMeans(select(., reading1_waist, reading2_waist, reading3_waist), na.rm=TRUE), 2)</t>
-  </si>
-  <si>
-    <t>round(rowMeans(select(., bp1systolic1, bp1systolic2, bp1systolic3), na.rm=TRUE), 2)</t>
-  </si>
-  <si>
-    <t>round(rowMeans(select(., bp1diastolic1, bp1diastolic2, bp1diastolic3), na.rm=TRUE), 2)</t>
-  </si>
-  <si>
-    <t>round(rowMeans(select(., bp1hr1, bp1hr2, bp1hr3), na.rm=TRUE), 2)</t>
   </si>
   <si>
     <t>case_when(
@@ -1731,13 +1722,6 @@
     <t>not in report, only edited data dict. Must confirm</t>
   </si>
   <si>
-    <t>rowSums(mutate(.,
-temp_b3 = b3*(300*0.05*0.7893),
-temp_b4 = b4*(175*0.12*0.7893),
-temp_b5 = b5*(35*0.4*0.7893)) %&gt;%
-select(temp_b3, temp_b4, temp_b5), na.rm = TRUE)</t>
-  </si>
-  <si>
     <t>confirm conversion</t>
   </si>
   <si>
@@ -1882,6 +1866,26 @@
 temp_l10min = ifelse(!is.na(l10min),l10min/60,NA),
 temp_l12min = ifelse(!is.na(l12min),l12min/60,NA)) %&gt;%
 select(temp_l10min, l10hr, temp_l12min, l12hr), na.rm = TRUE))</t>
+  </si>
+  <si>
+    <t>case_when(bp1diastolic3 == 0 ~ round(rowMeans(select(., bp1diastolic1, bp1diastolic2), na.rm=TRUE), 2);
+ELSE ~  round(rowMeans(select(., bp1diastolic1, bp1diastolic2, bp1diastolic3), na.rm=TRUE), 2))</t>
+  </si>
+  <si>
+    <t>case_when(bp1systolic3 == 0 ~ round(rowMeans(select(., bp1systolic1, bp1systolic2), na.rm=TRUE), 2);
+ELSE ~ round(rowMeans(select(., bp1systolic1, bp1systolic2, bp1systolic3), na.rm=TRUE), 2))</t>
+  </si>
+  <si>
+    <t>case_when(bp1hr3 == 0 ~ round(rowMeans(select(., bp1hr1, bp1hr2), na.rm=TRUE), 2);
+ELSE ~ round(rowMeans(select(., bp1hr1, bp1hr2, bp1hr3), na.rm=TRUE), 2))</t>
+  </si>
+  <si>
+    <t>case_when(is.na(b3) &amp; is.na(b4) &amp; is.na(b5) ~ NA;
+ELSE ~ rowSums(mutate(.,
+temp_b3 = b3*(300*0.05*0.7893),
+temp_b4 = b4*(175*0.12*0.7893),
+temp_b5 = b5*(35*0.4*0.7893)) %&gt;%
+select(temp_b3, temp_b4, temp_b5), na.rm = TRUE))</t>
   </si>
 </sst>
 </file>
@@ -2360,10 +2364,10 @@
   <dimension ref="A1:AD84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="S73" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="S29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W77" sqref="W77"/>
+      <selection pane="bottomRight" activeCell="W41" sqref="W41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="54.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2420,19 +2424,19 @@
         <v>10</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="M1" s="9" t="s">
         <v>11</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="Q1" s="4" t="s">
         <v>12</v>
@@ -2456,25 +2460,25 @@
         <v>18</v>
       </c>
       <c r="X1" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="Y1" t="s">
         <v>19</v>
       </c>
       <c r="Z1" t="s">
+        <v>485</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>486</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>487</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>488</v>
+      </c>
+      <c r="AD1" t="s">
         <v>489</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>490</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>491</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>492</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
@@ -2500,7 +2504,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="11"/>
       <c r="J2" s="1" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>296</v>
@@ -2523,7 +2527,7 @@
         <v>26</v>
       </c>
       <c r="W2" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="3" spans="1:30" ht="75" x14ac:dyDescent="0.25">
@@ -2551,7 +2555,7 @@
       </c>
       <c r="I3" s="11"/>
       <c r="J3" s="1" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>313</v>
@@ -2576,10 +2580,10 @@
         <v>32</v>
       </c>
       <c r="W3" t="s">
+        <v>436</v>
+      </c>
+      <c r="X3" t="s">
         <v>439</v>
-      </c>
-      <c r="X3" t="s">
-        <v>442</v>
       </c>
       <c r="Y3" s="14" t="s">
         <v>314</v>
@@ -2622,7 +2626,7 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="Q4" s="6" t="s">
         <v>317</v>
@@ -2678,7 +2682,7 @@
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>23</v>
@@ -2738,7 +2742,7 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="Q6" s="6" t="s">
         <v>323</v>
@@ -2758,7 +2762,7 @@
         <v>324</v>
       </c>
       <c r="X6" s="14" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="Y6" t="s">
         <v>288</v>
@@ -2801,7 +2805,7 @@
       <c r="N7" s="1"/>
       <c r="O7" s="6"/>
       <c r="P7" s="1" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="Q7" s="1" t="s">
         <v>327</v>
@@ -2823,7 +2827,7 @@
         <v>3</v>
       </c>
       <c r="X7" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="Y7" t="s">
         <v>329</v>
@@ -2866,7 +2870,7 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="Q8" s="6" t="s">
         <v>332</v>
@@ -2970,7 +2974,7 @@
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="Q10" s="6" t="s">
         <v>335</v>
@@ -2990,10 +2994,10 @@
         <v>61</v>
       </c>
       <c r="X10" s="14" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="Z10" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="11" spans="1:30" ht="180" x14ac:dyDescent="0.25">
@@ -3031,7 +3035,7 @@
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="Q11" s="6" t="s">
         <v>338</v>
@@ -3051,7 +3055,7 @@
         <v>339</v>
       </c>
       <c r="Z11" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="12" spans="1:30" ht="128.25" x14ac:dyDescent="0.25">
@@ -3091,7 +3095,7 @@
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="Q12" s="6" t="s">
         <v>332</v>
@@ -3111,7 +3115,7 @@
         <v>340</v>
       </c>
       <c r="Z12" s="14" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="13" spans="1:30" ht="85.5" x14ac:dyDescent="0.25">
@@ -3151,7 +3155,7 @@
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="Q13" s="6" t="s">
         <v>343</v>
@@ -3208,7 +3212,7 @@
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="Q14" s="6" t="s">
         <v>343</v>
@@ -3281,7 +3285,7 @@
         <v>2</v>
       </c>
       <c r="X15" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="Y15" t="s">
         <v>346</v>
@@ -3735,7 +3739,7 @@
         <v>61</v>
       </c>
       <c r="X23" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="Y23" t="s">
         <v>358</v>
@@ -3788,13 +3792,13 @@
         <v>61</v>
       </c>
       <c r="X24" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="Y24" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -3842,13 +3846,13 @@
         <v>50</v>
       </c>
       <c r="V25" t="s">
-        <v>32</v>
-      </c>
-      <c r="W25" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="W25" s="14" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -3896,13 +3900,13 @@
         <v>50</v>
       </c>
       <c r="V26" t="s">
-        <v>32</v>
-      </c>
-      <c r="W26" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="W26" s="14" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -3954,8 +3958,8 @@
       <c r="V27" t="s">
         <v>32</v>
       </c>
-      <c r="W27" t="s">
-        <v>425</v>
+      <c r="W27" s="14" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
@@ -4057,10 +4061,10 @@
         <v>205</v>
       </c>
       <c r="W29" s="14" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="X29" s="14" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="Y29" t="s">
         <v>367</v>
@@ -4169,10 +4173,10 @@
         <v>32</v>
       </c>
       <c r="W31" s="17" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="X31" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="Y31" t="s">
         <v>292</v>
@@ -4233,7 +4237,7 @@
         <v>45</v>
       </c>
       <c r="X32" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.25">
@@ -4291,7 +4295,7 @@
         <v>45</v>
       </c>
       <c r="X33" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.25">
@@ -4349,7 +4353,7 @@
         <v>45</v>
       </c>
       <c r="X34" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.25">
@@ -4388,7 +4392,7 @@
       </c>
       <c r="N35" s="1"/>
       <c r="O35" s="1" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
@@ -4408,7 +4412,7 @@
         <v>32</v>
       </c>
       <c r="W35" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.25">
@@ -4463,10 +4467,10 @@
         <v>32</v>
       </c>
       <c r="W36" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="X36" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.25">
@@ -4554,7 +4558,7 @@
       </c>
       <c r="N38" s="1"/>
       <c r="O38" s="1" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="P38" s="1" t="s">
         <v>44</v>
@@ -4577,7 +4581,7 @@
         <v>61</v>
       </c>
       <c r="X38" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="Y38" t="s">
         <v>302</v>
@@ -4668,7 +4672,7 @@
       </c>
       <c r="N40" s="1"/>
       <c r="O40" s="1" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="P40" s="1" t="s">
         <v>44</v>
@@ -4779,7 +4783,7 @@
       </c>
       <c r="N42" s="1"/>
       <c r="O42" s="1" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="P42" s="1" t="s">
         <v>44</v>
@@ -4802,7 +4806,7 @@
         <v>45</v>
       </c>
       <c r="X42" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="Y42" t="s">
         <v>377</v>
@@ -4857,13 +4861,13 @@
         <v>50</v>
       </c>
       <c r="V43" t="s">
-        <v>32</v>
+        <v>205</v>
       </c>
       <c r="W43" s="14" t="s">
-        <v>463</v>
+        <v>497</v>
       </c>
       <c r="X43" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="Y43" s="14" t="s">
         <v>385</v>
@@ -4891,7 +4895,7 @@
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="15" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>386</v>
@@ -4906,7 +4910,7 @@
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
       <c r="P44" s="1" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="Q44" s="6" t="s">
         <v>389</v>
@@ -5007,7 +5011,7 @@
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="15" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="J46" s="6" t="s">
         <v>391</v>
@@ -5146,7 +5150,7 @@
         <v>61</v>
       </c>
       <c r="X48" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="Y48" t="s">
         <v>402</v>
@@ -5200,7 +5204,7 @@
         <v>61</v>
       </c>
       <c r="X49" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="Y49" t="s">
         <v>198</v>
@@ -5289,7 +5293,7 @@
       <c r="O51" s="1"/>
       <c r="P51" s="1"/>
       <c r="Q51" s="1" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="R51" s="1"/>
       <c r="S51" s="1"/>
@@ -5407,7 +5411,7 @@
         <v>61</v>
       </c>
       <c r="X53" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="Y53" t="s">
         <v>403</v>
@@ -5498,13 +5502,13 @@
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
       <c r="M55" s="11" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="N55" s="1"/>
       <c r="O55" s="1"/>
       <c r="P55" s="1"/>
       <c r="Q55" s="6" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="R55" s="1"/>
       <c r="S55" s="1"/>
@@ -5518,7 +5522,7 @@
         <v>38</v>
       </c>
       <c r="W55" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="Y55" t="s">
         <v>198</v>
@@ -5554,13 +5558,13 @@
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
       <c r="M56" s="11" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="N56" s="1"/>
       <c r="O56" s="1"/>
       <c r="P56" s="1"/>
       <c r="Q56" s="6" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="R56" s="1"/>
       <c r="S56" s="1"/>
@@ -5574,7 +5578,7 @@
         <v>38</v>
       </c>
       <c r="W56" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="Y56" t="s">
         <v>198</v>
@@ -5610,13 +5614,13 @@
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
       <c r="M57" s="11" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="N57" s="1"/>
       <c r="O57" s="1"/>
       <c r="P57" s="1"/>
       <c r="Q57" s="6" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="R57" s="1"/>
       <c r="S57" s="1"/>
@@ -5630,7 +5634,7 @@
         <v>38</v>
       </c>
       <c r="W57" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="Y57" t="s">
         <v>198</v>
@@ -6112,7 +6116,7 @@
         <v>61</v>
       </c>
       <c r="X67" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="Y67" t="s">
         <v>198</v>
@@ -6167,7 +6171,7 @@
         <v>61</v>
       </c>
       <c r="X68" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="Y68" t="s">
         <v>198</v>
@@ -6222,7 +6226,7 @@
         <v>61</v>
       </c>
       <c r="X69" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="Y69" t="s">
         <v>198</v>
@@ -6274,10 +6278,10 @@
         <v>205</v>
       </c>
       <c r="W70" s="14" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="X70" s="14" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="Y70" t="s">
         <v>198</v>
@@ -6329,7 +6333,7 @@
         <v>205</v>
       </c>
       <c r="W71" s="14" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="Y71" t="s">
         <v>198</v>
@@ -6381,7 +6385,7 @@
         <v>205</v>
       </c>
       <c r="W72" s="14" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="Y72" t="s">
         <v>198</v>
@@ -6580,7 +6584,7 @@
         <v>32</v>
       </c>
       <c r="W76" s="14" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="Y76" t="s">
         <v>408</v>
@@ -6630,10 +6634,10 @@
         <v>205</v>
       </c>
       <c r="W77" s="14" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="X77" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="Y77" t="s">
         <v>408</v>
@@ -6673,7 +6677,7 @@
       <c r="O78" s="1"/>
       <c r="P78" s="1"/>
       <c r="Q78" s="1" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="R78" s="1"/>
       <c r="S78" s="6"/>
@@ -6687,7 +6691,7 @@
         <v>205</v>
       </c>
       <c r="W78" s="14" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="Y78" t="s">
         <v>198</v>
@@ -6773,7 +6777,7 @@
         <v>189</v>
       </c>
       <c r="J80" s="6" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="K80" s="1"/>
       <c r="L80" s="1"/>
@@ -6784,7 +6788,7 @@
       <c r="Q80" s="1"/>
       <c r="R80" s="1"/>
       <c r="S80" s="6" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="T80" s="7" t="s">
         <v>24</v>
@@ -6796,7 +6800,7 @@
         <v>205</v>
       </c>
       <c r="W80" s="14" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="Y80" t="s">
         <v>198</v>
@@ -6832,13 +6836,13 @@
       <c r="K81" s="1"/>
       <c r="L81" s="1"/>
       <c r="M81" s="15" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="N81" s="1"/>
       <c r="O81" s="1"/>
       <c r="P81" s="1"/>
       <c r="Q81" s="1" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="R81" s="1"/>
       <c r="S81" s="6"/>
@@ -6852,7 +6856,7 @@
         <v>205</v>
       </c>
       <c r="W81" s="14" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="82" spans="1:25" ht="409.5" x14ac:dyDescent="0.25">
@@ -6880,7 +6884,7 @@
         <v>189</v>
       </c>
       <c r="J82" s="6" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="K82" s="1"/>
       <c r="L82" s="1"/>
@@ -6891,7 +6895,7 @@
       <c r="Q82" s="1"/>
       <c r="R82" s="1"/>
       <c r="S82" s="6" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="T82" s="7" t="s">
         <v>24</v>
@@ -6903,7 +6907,7 @@
         <v>205</v>
       </c>
       <c r="W82" s="14" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="Y82" t="s">
         <v>198</v>

</xml_diff>

<commit_message>
correct resting heart rate
</commit_message>
<xml_diff>
--- a/data_processing_elements-SHS.xlsx
+++ b/data_processing_elements-SHS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D38B06AB-1D90-4985-92B5-232B53A04D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D689B4-423B-4235-AFB1-6093CBF8421C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
@@ -1242,9 +1242,6 @@
   </si>
   <si>
     <t>Diastolic blood pressure - 1st measurement; Diastolic blood pressure - 2nd measurement; Diastolic blood pressure - 3rd measurement</t>
-  </si>
-  <si>
-    <t>bp1hr1; bp1hr2; bp1hr3</t>
   </si>
   <si>
     <t>Pulse rate</t>
@@ -1886,6 +1883,11 @@
 temp_b4 = b4*(175*0.12*0.7893),
 temp_b5 = b5*(35*0.4*0.7893)) %&gt;%
 select(temp_b3, temp_b4, temp_b5), na.rm = TRUE))</t>
+  </si>
+  <si>
+    <t>bp1hr1;
+bp1hr2; 
+bp1hr3</t>
   </si>
 </sst>
 </file>
@@ -2364,10 +2366,10 @@
   <dimension ref="A1:AD84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="S29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="Q14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W41" sqref="W41"/>
+      <selection pane="bottomRight" activeCell="U32" sqref="U32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="54.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2424,19 +2426,19 @@
         <v>10</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="M1" s="9" t="s">
         <v>11</v>
       </c>
       <c r="N1" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="O1" s="4" t="s">
         <v>481</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>482</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>483</v>
       </c>
       <c r="Q1" s="4" t="s">
         <v>12</v>
@@ -2460,25 +2462,25 @@
         <v>18</v>
       </c>
       <c r="X1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="Y1" t="s">
         <v>19</v>
       </c>
       <c r="Z1" t="s">
+        <v>484</v>
+      </c>
+      <c r="AA1" t="s">
         <v>485</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>486</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>487</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>488</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
@@ -2504,7 +2506,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="11"/>
       <c r="J2" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>296</v>
@@ -2527,7 +2529,7 @@
         <v>26</v>
       </c>
       <c r="W2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="3" spans="1:30" ht="75" x14ac:dyDescent="0.25">
@@ -2555,7 +2557,7 @@
       </c>
       <c r="I3" s="11"/>
       <c r="J3" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>313</v>
@@ -2580,10 +2582,10 @@
         <v>32</v>
       </c>
       <c r="W3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="X3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="Y3" s="14" t="s">
         <v>314</v>
@@ -2626,7 +2628,7 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="Q4" s="6" t="s">
         <v>317</v>
@@ -2682,7 +2684,7 @@
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>23</v>
@@ -2742,7 +2744,7 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="Q6" s="6" t="s">
         <v>323</v>
@@ -2762,7 +2764,7 @@
         <v>324</v>
       </c>
       <c r="X6" s="14" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="Y6" t="s">
         <v>288</v>
@@ -2805,7 +2807,7 @@
       <c r="N7" s="1"/>
       <c r="O7" s="6"/>
       <c r="P7" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="Q7" s="1" t="s">
         <v>327</v>
@@ -2827,7 +2829,7 @@
         <v>3</v>
       </c>
       <c r="X7" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="Y7" t="s">
         <v>329</v>
@@ -2870,7 +2872,7 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="Q8" s="6" t="s">
         <v>332</v>
@@ -2974,7 +2976,7 @@
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="Q10" s="6" t="s">
         <v>335</v>
@@ -2994,10 +2996,10 @@
         <v>61</v>
       </c>
       <c r="X10" s="14" t="s">
+        <v>443</v>
+      </c>
+      <c r="Z10" t="s">
         <v>444</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="11" spans="1:30" ht="180" x14ac:dyDescent="0.25">
@@ -3035,7 +3037,7 @@
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="Q11" s="6" t="s">
         <v>338</v>
@@ -3055,7 +3057,7 @@
         <v>339</v>
       </c>
       <c r="Z11" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="12" spans="1:30" ht="128.25" x14ac:dyDescent="0.25">
@@ -3095,7 +3097,7 @@
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="Q12" s="6" t="s">
         <v>332</v>
@@ -3115,7 +3117,7 @@
         <v>340</v>
       </c>
       <c r="Z12" s="14" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="13" spans="1:30" ht="85.5" x14ac:dyDescent="0.25">
@@ -3155,7 +3157,7 @@
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="Q13" s="6" t="s">
         <v>343</v>
@@ -3212,7 +3214,7 @@
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="Q14" s="6" t="s">
         <v>343</v>
@@ -3285,7 +3287,7 @@
         <v>2</v>
       </c>
       <c r="X15" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="Y15" t="s">
         <v>346</v>
@@ -3601,7 +3603,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="11"/>
       <c r="J21" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>354</v>
@@ -3632,7 +3634,7 @@
         <v>32</v>
       </c>
       <c r="W21" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="Y21" t="s">
         <v>356</v>
@@ -3663,7 +3665,7 @@
         <v>94</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -3739,7 +3741,7 @@
         <v>61</v>
       </c>
       <c r="X23" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="Y23" t="s">
         <v>358</v>
@@ -3792,7 +3794,7 @@
         <v>61</v>
       </c>
       <c r="X24" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="Y24" t="s">
         <v>358</v>
@@ -3849,7 +3851,7 @@
         <v>205</v>
       </c>
       <c r="W25" s="14" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="26" spans="1:25" ht="60" x14ac:dyDescent="0.25">
@@ -3903,7 +3905,7 @@
         <v>205</v>
       </c>
       <c r="W26" s="14" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="27" spans="1:25" ht="45" x14ac:dyDescent="0.25">
@@ -3930,11 +3932,11 @@
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="11"/>
-      <c r="J27" s="1" t="s">
+      <c r="J27" s="6" t="s">
+        <v>497</v>
+      </c>
+      <c r="K27" s="1" t="s">
         <v>363</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>364</v>
       </c>
       <c r="L27" s="1"/>
       <c r="M27" s="11" t="s">
@@ -3956,10 +3958,10 @@
         <v>50</v>
       </c>
       <c r="V27" t="s">
-        <v>32</v>
+        <v>205</v>
       </c>
       <c r="W27" s="14" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
@@ -4036,10 +4038,10 @@
         <v>129</v>
       </c>
       <c r="J29" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="K29" s="1" t="s">
         <v>365</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>366</v>
       </c>
       <c r="L29" s="1"/>
       <c r="M29" s="11"/>
@@ -4061,13 +4063,13 @@
         <v>205</v>
       </c>
       <c r="W29" s="14" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="X29" s="14" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="Y29" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
@@ -4144,7 +4146,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="11"/>
       <c r="J31" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>307</v>
@@ -4173,10 +4175,10 @@
         <v>32</v>
       </c>
       <c r="W31" s="17" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="X31" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="Y31" t="s">
         <v>292</v>
@@ -4237,7 +4239,7 @@
         <v>45</v>
       </c>
       <c r="X32" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.25">
@@ -4295,7 +4297,7 @@
         <v>45</v>
       </c>
       <c r="X33" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.25">
@@ -4353,7 +4355,7 @@
         <v>45</v>
       </c>
       <c r="X34" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.25">
@@ -4381,18 +4383,18 @@
       <c r="H35" s="1"/>
       <c r="I35" s="11"/>
       <c r="J35" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="L35" s="1"/>
       <c r="M35" s="11" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="N35" s="1"/>
       <c r="O35" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
@@ -4412,7 +4414,7 @@
         <v>32</v>
       </c>
       <c r="W35" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.25">
@@ -4440,7 +4442,7 @@
       <c r="H36" s="1"/>
       <c r="I36" s="11"/>
       <c r="J36" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>146</v>
@@ -4467,10 +4469,10 @@
         <v>32</v>
       </c>
       <c r="W36" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="X36" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.25">
@@ -4547,18 +4549,18 @@
       <c r="H38" s="1"/>
       <c r="I38" s="11"/>
       <c r="J38" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="K38" s="1" t="s">
         <v>372</v>
-      </c>
-      <c r="K38" s="1" t="s">
-        <v>373</v>
       </c>
       <c r="L38" s="1"/>
       <c r="M38" s="11" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="N38" s="1"/>
       <c r="O38" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="P38" s="1" t="s">
         <v>44</v>
@@ -4581,7 +4583,7 @@
         <v>61</v>
       </c>
       <c r="X38" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="Y38" t="s">
         <v>302</v>
@@ -4661,18 +4663,18 @@
       <c r="H40" s="1"/>
       <c r="I40" s="11"/>
       <c r="J40" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="L40" s="1"/>
       <c r="M40" s="11" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="N40" s="1"/>
       <c r="O40" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="P40" s="1" t="s">
         <v>44</v>
@@ -4695,7 +4697,7 @@
         <v>45</v>
       </c>
       <c r="Y40" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="41" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
@@ -4772,18 +4774,18 @@
       <c r="H42" s="1"/>
       <c r="I42" s="11"/>
       <c r="J42" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="K42" s="1" t="s">
         <v>378</v>
-      </c>
-      <c r="K42" s="1" t="s">
-        <v>379</v>
       </c>
       <c r="L42" s="1"/>
       <c r="M42" s="11" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="N42" s="1"/>
       <c r="O42" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="P42" s="1" t="s">
         <v>44</v>
@@ -4806,10 +4808,10 @@
         <v>45</v>
       </c>
       <c r="X42" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="Y42" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="43" spans="1:25" ht="90" x14ac:dyDescent="0.25">
@@ -4837,14 +4839,14 @@
       <c r="H43" s="1"/>
       <c r="I43" s="11"/>
       <c r="J43" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="K43" s="6" t="s">
         <v>381</v>
-      </c>
-      <c r="K43" s="6" t="s">
-        <v>382</v>
       </c>
       <c r="L43" s="1"/>
       <c r="M43" s="15" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
@@ -4852,7 +4854,7 @@
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
       <c r="S43" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="T43" s="7" t="s">
         <v>24</v>
@@ -4864,13 +4866,13 @@
         <v>205</v>
       </c>
       <c r="W43" s="14" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="X43" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="Y43" s="14" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="44" spans="1:25" ht="142.5" x14ac:dyDescent="0.25">
@@ -4895,25 +4897,25 @@
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="15" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="J44" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="K44" s="1" t="s">
         <v>386</v>
-      </c>
-      <c r="K44" s="1" t="s">
-        <v>387</v>
       </c>
       <c r="L44" s="1"/>
       <c r="M44" s="11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
       <c r="P44" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="Q44" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="R44" s="1"/>
       <c r="S44" s="1" t="s">
@@ -4929,7 +4931,7 @@
         <v>38</v>
       </c>
       <c r="W44" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="45" spans="1:25" ht="75" x14ac:dyDescent="0.25">
@@ -4957,24 +4959,24 @@
         <v>177</v>
       </c>
       <c r="J45" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="K45" s="6" t="s">
         <v>391</v>
-      </c>
-      <c r="K45" s="6" t="s">
-        <v>392</v>
       </c>
       <c r="L45" s="1"/>
       <c r="M45" s="15" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
       <c r="P45" s="1"/>
       <c r="Q45" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="R45" s="1"/>
       <c r="S45" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="T45" s="1" t="s">
         <v>24</v>
@@ -4986,7 +4988,7 @@
         <v>205</v>
       </c>
       <c r="W45" s="14" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="46" spans="1:25" ht="71.25" x14ac:dyDescent="0.25">
@@ -5011,23 +5013,23 @@
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="J46" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="K46" s="6" t="s">
         <v>391</v>
-      </c>
-      <c r="K46" s="6" t="s">
-        <v>392</v>
       </c>
       <c r="L46" s="1"/>
       <c r="M46" s="15" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
       <c r="P46" s="1"/>
       <c r="Q46" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="R46" s="1"/>
       <c r="S46" s="1"/>
@@ -5069,14 +5071,14 @@
       <c r="H47" s="1"/>
       <c r="I47" s="11"/>
       <c r="J47" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="K47" s="1" t="s">
         <v>397</v>
-      </c>
-      <c r="K47" s="1" t="s">
-        <v>398</v>
       </c>
       <c r="L47" s="1"/>
       <c r="M47" s="11" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
@@ -5085,7 +5087,7 @@
         <v>44</v>
       </c>
       <c r="R47" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="S47" s="1"/>
       <c r="T47" s="1" t="s">
@@ -5098,7 +5100,7 @@
         <v>32</v>
       </c>
       <c r="W47" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="48" spans="1:25" ht="51" x14ac:dyDescent="0.25">
@@ -5150,10 +5152,10 @@
         <v>61</v>
       </c>
       <c r="X48" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="Y48" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="49" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
@@ -5204,7 +5206,7 @@
         <v>61</v>
       </c>
       <c r="X49" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="Y49" t="s">
         <v>198</v>
@@ -5284,7 +5286,7 @@
         <v>189</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
@@ -5293,7 +5295,7 @@
       <c r="O51" s="1"/>
       <c r="P51" s="1"/>
       <c r="Q51" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="R51" s="1"/>
       <c r="S51" s="1"/>
@@ -5411,10 +5413,10 @@
         <v>61</v>
       </c>
       <c r="X53" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="Y53" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="54" spans="1:25" ht="28.5" x14ac:dyDescent="0.25">
@@ -5442,20 +5444,20 @@
         <v>189</v>
       </c>
       <c r="J54" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="K54" s="1" t="s">
         <v>404</v>
-      </c>
-      <c r="K54" s="1" t="s">
-        <v>405</v>
       </c>
       <c r="L54" s="1"/>
       <c r="M54" s="11" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="N54" s="1"/>
       <c r="O54" s="1"/>
       <c r="P54" s="1"/>
       <c r="Q54" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="R54" s="1"/>
       <c r="S54" s="1"/>
@@ -5497,18 +5499,18 @@
         <v>189</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
       <c r="M55" s="11" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="N55" s="1"/>
       <c r="O55" s="1"/>
       <c r="P55" s="1"/>
       <c r="Q55" s="6" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R55" s="1"/>
       <c r="S55" s="1"/>
@@ -5522,7 +5524,7 @@
         <v>38</v>
       </c>
       <c r="W55" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="Y55" t="s">
         <v>198</v>
@@ -5553,18 +5555,18 @@
         <v>189</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
       <c r="M56" s="11" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N56" s="1"/>
       <c r="O56" s="1"/>
       <c r="P56" s="1"/>
       <c r="Q56" s="6" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R56" s="1"/>
       <c r="S56" s="1"/>
@@ -5578,7 +5580,7 @@
         <v>38</v>
       </c>
       <c r="W56" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="Y56" t="s">
         <v>198</v>
@@ -5609,18 +5611,18 @@
         <v>189</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
       <c r="M57" s="11" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="N57" s="1"/>
       <c r="O57" s="1"/>
       <c r="P57" s="1"/>
       <c r="Q57" s="6" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="R57" s="1"/>
       <c r="S57" s="1"/>
@@ -5634,7 +5636,7 @@
         <v>38</v>
       </c>
       <c r="W57" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="Y57" t="s">
         <v>198</v>
@@ -6116,7 +6118,7 @@
         <v>61</v>
       </c>
       <c r="X67" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="Y67" t="s">
         <v>198</v>
@@ -6171,7 +6173,7 @@
         <v>61</v>
       </c>
       <c r="X68" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="Y68" t="s">
         <v>198</v>
@@ -6226,13 +6228,13 @@
         <v>61</v>
       </c>
       <c r="X69" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="Y69" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="70" spans="1:25" ht="195" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:25" ht="150" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -6257,7 +6259,7 @@
         <v>241</v>
       </c>
       <c r="J70" s="6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="K70" s="1"/>
       <c r="L70" s="1"/>
@@ -6278,16 +6280,16 @@
         <v>205</v>
       </c>
       <c r="W70" s="14" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="X70" s="14" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="Y70" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="71" spans="1:25" ht="150" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:25" ht="135" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -6312,7 +6314,7 @@
         <v>241</v>
       </c>
       <c r="J71" s="6" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>
@@ -6333,13 +6335,13 @@
         <v>205</v>
       </c>
       <c r="W71" s="14" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="Y71" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="72" spans="1:25" ht="150" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:25" ht="135" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -6364,7 +6366,7 @@
         <v>241</v>
       </c>
       <c r="J72" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="K72" s="1"/>
       <c r="L72" s="1"/>
@@ -6385,7 +6387,7 @@
         <v>205</v>
       </c>
       <c r="W72" s="14" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="Y72" t="s">
         <v>198</v>
@@ -6563,7 +6565,7 @@
       <c r="H76" s="1"/>
       <c r="I76" s="11"/>
       <c r="J76" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="K76" s="1"/>
       <c r="L76" s="1"/>
@@ -6584,10 +6586,10 @@
         <v>32</v>
       </c>
       <c r="W76" s="14" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="Y76" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="77" spans="1:25" ht="390" x14ac:dyDescent="0.25">
@@ -6613,7 +6615,7 @@
         <v>264</v>
       </c>
       <c r="J77" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="K77" s="1"/>
       <c r="L77" s="1"/>
@@ -6634,13 +6636,13 @@
         <v>205</v>
       </c>
       <c r="W77" s="14" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="X77" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="Y77" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="78" spans="1:25" ht="75" x14ac:dyDescent="0.25">
@@ -6668,7 +6670,7 @@
         <v>268</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="K78" s="1"/>
       <c r="L78" s="1"/>
@@ -6677,7 +6679,7 @@
       <c r="O78" s="1"/>
       <c r="P78" s="1"/>
       <c r="Q78" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="R78" s="1"/>
       <c r="S78" s="6"/>
@@ -6691,7 +6693,7 @@
         <v>205</v>
       </c>
       <c r="W78" s="14" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="Y78" t="s">
         <v>198</v>
@@ -6749,7 +6751,7 @@
         <v>61</v>
       </c>
       <c r="Y79" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="80" spans="1:25" ht="409.5" x14ac:dyDescent="0.25">
@@ -6777,7 +6779,7 @@
         <v>189</v>
       </c>
       <c r="J80" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K80" s="1"/>
       <c r="L80" s="1"/>
@@ -6788,7 +6790,7 @@
       <c r="Q80" s="1"/>
       <c r="R80" s="1"/>
       <c r="S80" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="T80" s="7" t="s">
         <v>24</v>
@@ -6800,7 +6802,7 @@
         <v>205</v>
       </c>
       <c r="W80" s="14" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="Y80" t="s">
         <v>198</v>
@@ -6831,18 +6833,18 @@
         <v>189</v>
       </c>
       <c r="J81" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="K81" s="1"/>
       <c r="L81" s="1"/>
       <c r="M81" s="15" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="N81" s="1"/>
       <c r="O81" s="1"/>
       <c r="P81" s="1"/>
       <c r="Q81" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="R81" s="1"/>
       <c r="S81" s="6"/>
@@ -6856,7 +6858,7 @@
         <v>205</v>
       </c>
       <c r="W81" s="14" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="82" spans="1:25" ht="409.5" x14ac:dyDescent="0.25">
@@ -6884,7 +6886,7 @@
         <v>189</v>
       </c>
       <c r="J82" s="6" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="K82" s="1"/>
       <c r="L82" s="1"/>
@@ -6895,7 +6897,7 @@
       <c r="Q82" s="1"/>
       <c r="R82" s="1"/>
       <c r="S82" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="T82" s="7" t="s">
         <v>24</v>
@@ -6907,7 +6909,7 @@
         <v>205</v>
       </c>
       <c r="W82" s="14" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="Y82" t="s">
         <v>198</v>

</xml_diff>

<commit_message>
vccorrect smoking quantity and hear rate
</commit_message>
<xml_diff>
--- a/data_processing_elements-SHS.xlsx
+++ b/data_processing_elements-SHS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D689B4-423B-4235-AFB1-6093CBF8421C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{100ECC84-4E17-4B36-964F-3F4494B42AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
@@ -1379,9 +1379,6 @@
   </si>
   <si>
     <t>number of cigarettes per day</t>
-  </si>
-  <si>
-    <t>c7*7</t>
   </si>
   <si>
     <t>Is this variable available, if so, please provide us the information</t>
@@ -1865,16 +1862,8 @@
 select(temp_l10min, l10hr, temp_l12min, l12hr), na.rm = TRUE))</t>
   </si>
   <si>
-    <t>case_when(bp1diastolic3 == 0 ~ round(rowMeans(select(., bp1diastolic1, bp1diastolic2), na.rm=TRUE), 2);
-ELSE ~  round(rowMeans(select(., bp1diastolic1, bp1diastolic2, bp1diastolic3), na.rm=TRUE), 2))</t>
-  </si>
-  <si>
     <t>case_when(bp1systolic3 == 0 ~ round(rowMeans(select(., bp1systolic1, bp1systolic2), na.rm=TRUE), 2);
 ELSE ~ round(rowMeans(select(., bp1systolic1, bp1systolic2, bp1systolic3), na.rm=TRUE), 2))</t>
-  </si>
-  <si>
-    <t>case_when(bp1hr3 == 0 ~ round(rowMeans(select(., bp1hr1, bp1hr2), na.rm=TRUE), 2);
-ELSE ~ round(rowMeans(select(., bp1hr1, bp1hr2, bp1hr3), na.rm=TRUE), 2))</t>
   </si>
   <si>
     <t>case_when(is.na(b3) &amp; is.na(b4) &amp; is.na(b5) ~ NA;
@@ -1885,9 +1874,20 @@
 select(temp_b3, temp_b4, temp_b5), na.rm = TRUE))</t>
   </si>
   <si>
-    <t>bp1hr1;
-bp1hr2; 
-bp1hr3</t>
+    <t>case_when(bp1diastolic3 == 0 ~ round(rowMeans(select(., bp1diastolic1, bp1diastolic2), na.rm=TRUE), 2);
+ELSE ~ round(rowMeans(select(., bp1diastolic1, bp1diastolic2, bp1diastolic3), na.rm=TRUE), 2))</t>
+  </si>
+  <si>
+    <t>bp1hr1; bp1hr2; bp1hr3</t>
+  </si>
+  <si>
+    <t>case_when(bp1hr1 == 0 &amp; bp1hr2 == 0 &amp; bp1hr3 == 0 ~ NA; 
+bp1hr3 == 0 ~ round(rowMeans(select(., bp1hr1, bp1hr2), na.rm=TRUE), 2);
+ELSE ~ round(rowMeans(select(., bp1hr1, bp1hr2, bp1hr3), na.rm=TRUE), 2))</t>
+  </si>
+  <si>
+    <t>case_when(c7 == 999 ~ NA_integer_;
+ELSE ~ c7*7)</t>
   </si>
 </sst>
 </file>
@@ -2366,10 +2366,10 @@
   <dimension ref="A1:AD84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="Q14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="S17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U32" sqref="U32"/>
+      <selection pane="bottomRight" activeCell="W46" sqref="W46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="54.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2426,19 +2426,19 @@
         <v>10</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M1" s="9" t="s">
         <v>11</v>
       </c>
       <c r="N1" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="O1" s="4" t="s">
         <v>480</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>481</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>482</v>
       </c>
       <c r="Q1" s="4" t="s">
         <v>12</v>
@@ -2462,25 +2462,25 @@
         <v>18</v>
       </c>
       <c r="X1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="Y1" t="s">
         <v>19</v>
       </c>
       <c r="Z1" t="s">
+        <v>483</v>
+      </c>
+      <c r="AA1" t="s">
         <v>484</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>485</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>486</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>487</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
@@ -2506,7 +2506,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="11"/>
       <c r="J2" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>296</v>
@@ -2529,7 +2529,7 @@
         <v>26</v>
       </c>
       <c r="W2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="3" spans="1:30" ht="75" x14ac:dyDescent="0.25">
@@ -2557,7 +2557,7 @@
       </c>
       <c r="I3" s="11"/>
       <c r="J3" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>313</v>
@@ -2582,10 +2582,10 @@
         <v>32</v>
       </c>
       <c r="W3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="X3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="Y3" s="14" t="s">
         <v>314</v>
@@ -2628,7 +2628,7 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="Q4" s="6" t="s">
         <v>317</v>
@@ -2684,7 +2684,7 @@
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>23</v>
@@ -2744,7 +2744,7 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="Q6" s="6" t="s">
         <v>323</v>
@@ -2764,7 +2764,7 @@
         <v>324</v>
       </c>
       <c r="X6" s="14" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="Y6" t="s">
         <v>288</v>
@@ -2807,7 +2807,7 @@
       <c r="N7" s="1"/>
       <c r="O7" s="6"/>
       <c r="P7" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="Q7" s="1" t="s">
         <v>327</v>
@@ -2829,7 +2829,7 @@
         <v>3</v>
       </c>
       <c r="X7" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="Y7" t="s">
         <v>329</v>
@@ -2872,7 +2872,7 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="Q8" s="6" t="s">
         <v>332</v>
@@ -2976,7 +2976,7 @@
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="Q10" s="6" t="s">
         <v>335</v>
@@ -2996,10 +2996,10 @@
         <v>61</v>
       </c>
       <c r="X10" s="14" t="s">
+        <v>442</v>
+      </c>
+      <c r="Z10" t="s">
         <v>443</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="11" spans="1:30" ht="180" x14ac:dyDescent="0.25">
@@ -3037,7 +3037,7 @@
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="Q11" s="6" t="s">
         <v>338</v>
@@ -3057,7 +3057,7 @@
         <v>339</v>
       </c>
       <c r="Z11" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="12" spans="1:30" ht="128.25" x14ac:dyDescent="0.25">
@@ -3097,7 +3097,7 @@
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="Q12" s="6" t="s">
         <v>332</v>
@@ -3117,7 +3117,7 @@
         <v>340</v>
       </c>
       <c r="Z12" s="14" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="13" spans="1:30" ht="85.5" x14ac:dyDescent="0.25">
@@ -3157,7 +3157,7 @@
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="Q13" s="6" t="s">
         <v>343</v>
@@ -3214,7 +3214,7 @@
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="Q14" s="6" t="s">
         <v>343</v>
@@ -3287,7 +3287,7 @@
         <v>2</v>
       </c>
       <c r="X15" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="Y15" t="s">
         <v>346</v>
@@ -3603,7 +3603,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="11"/>
       <c r="J21" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>354</v>
@@ -3634,7 +3634,7 @@
         <v>32</v>
       </c>
       <c r="W21" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="Y21" t="s">
         <v>356</v>
@@ -3665,7 +3665,7 @@
         <v>94</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -3741,7 +3741,7 @@
         <v>61</v>
       </c>
       <c r="X23" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="Y23" t="s">
         <v>358</v>
@@ -3794,7 +3794,7 @@
         <v>61</v>
       </c>
       <c r="X24" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="Y24" t="s">
         <v>358</v>
@@ -3851,7 +3851,7 @@
         <v>205</v>
       </c>
       <c r="W25" s="14" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="26" spans="1:25" ht="60" x14ac:dyDescent="0.25">
@@ -3905,7 +3905,7 @@
         <v>205</v>
       </c>
       <c r="W26" s="14" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="27" spans="1:25" ht="45" x14ac:dyDescent="0.25">
@@ -3933,7 +3933,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="11"/>
       <c r="J27" s="6" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>363</v>
@@ -3958,10 +3958,10 @@
         <v>50</v>
       </c>
       <c r="V27" t="s">
-        <v>205</v>
+        <v>32</v>
       </c>
       <c r="W27" s="14" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
@@ -4063,10 +4063,10 @@
         <v>205</v>
       </c>
       <c r="W29" s="14" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="X29" s="14" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="Y29" t="s">
         <v>366</v>
@@ -4175,10 +4175,10 @@
         <v>32</v>
       </c>
       <c r="W31" s="17" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="X31" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="Y31" t="s">
         <v>292</v>
@@ -4239,7 +4239,7 @@
         <v>45</v>
       </c>
       <c r="X32" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.25">
@@ -4297,7 +4297,7 @@
         <v>45</v>
       </c>
       <c r="X33" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.25">
@@ -4355,7 +4355,7 @@
         <v>45</v>
       </c>
       <c r="X34" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.25">
@@ -4394,7 +4394,7 @@
       </c>
       <c r="N35" s="1"/>
       <c r="O35" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
@@ -4414,7 +4414,7 @@
         <v>32</v>
       </c>
       <c r="W35" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.25">
@@ -4469,10 +4469,10 @@
         <v>32</v>
       </c>
       <c r="W36" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="X36" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.25">
@@ -4560,7 +4560,7 @@
       </c>
       <c r="N38" s="1"/>
       <c r="O38" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="P38" s="1" t="s">
         <v>44</v>
@@ -4583,7 +4583,7 @@
         <v>61</v>
       </c>
       <c r="X38" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="Y38" t="s">
         <v>302</v>
@@ -4663,7 +4663,7 @@
       <c r="H40" s="1"/>
       <c r="I40" s="11"/>
       <c r="J40" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="K40" s="1" t="s">
         <v>374</v>
@@ -4674,7 +4674,7 @@
       </c>
       <c r="N40" s="1"/>
       <c r="O40" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="P40" s="1" t="s">
         <v>44</v>
@@ -4785,7 +4785,7 @@
       </c>
       <c r="N42" s="1"/>
       <c r="O42" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="P42" s="1" t="s">
         <v>44</v>
@@ -4808,7 +4808,7 @@
         <v>45</v>
       </c>
       <c r="X42" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="Y42" t="s">
         <v>376</v>
@@ -4866,10 +4866,10 @@
         <v>205</v>
       </c>
       <c r="W43" s="14" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="X43" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="Y43" s="14" t="s">
         <v>384</v>
@@ -4897,7 +4897,7 @@
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="15" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>385</v>
@@ -4912,7 +4912,7 @@
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
       <c r="P44" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="Q44" s="6" t="s">
         <v>388</v>
@@ -5013,7 +5013,7 @@
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="J46" s="6" t="s">
         <v>390</v>
@@ -5046,7 +5046,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -5097,10 +5097,10 @@
         <v>25</v>
       </c>
       <c r="V47" t="s">
-        <v>32</v>
-      </c>
-      <c r="W47" t="s">
-        <v>400</v>
+        <v>205</v>
+      </c>
+      <c r="W47" s="14" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="48" spans="1:25" ht="51" x14ac:dyDescent="0.25">
@@ -5152,10 +5152,10 @@
         <v>61</v>
       </c>
       <c r="X48" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="Y48" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="49" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
@@ -5206,7 +5206,7 @@
         <v>61</v>
       </c>
       <c r="X49" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="Y49" t="s">
         <v>198</v>
@@ -5286,7 +5286,7 @@
         <v>189</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
@@ -5295,7 +5295,7 @@
       <c r="O51" s="1"/>
       <c r="P51" s="1"/>
       <c r="Q51" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="R51" s="1"/>
       <c r="S51" s="1"/>
@@ -5413,10 +5413,10 @@
         <v>61</v>
       </c>
       <c r="X53" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="Y53" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="54" spans="1:25" ht="28.5" x14ac:dyDescent="0.25">
@@ -5444,20 +5444,20 @@
         <v>189</v>
       </c>
       <c r="J54" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="K54" s="1" t="s">
         <v>403</v>
-      </c>
-      <c r="K54" s="1" t="s">
-        <v>404</v>
       </c>
       <c r="L54" s="1"/>
       <c r="M54" s="11" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="N54" s="1"/>
       <c r="O54" s="1"/>
       <c r="P54" s="1"/>
       <c r="Q54" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="R54" s="1"/>
       <c r="S54" s="1"/>
@@ -5499,18 +5499,18 @@
         <v>189</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
       <c r="M55" s="11" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="N55" s="1"/>
       <c r="O55" s="1"/>
       <c r="P55" s="1"/>
       <c r="Q55" s="6" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="R55" s="1"/>
       <c r="S55" s="1"/>
@@ -5524,7 +5524,7 @@
         <v>38</v>
       </c>
       <c r="W55" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="Y55" t="s">
         <v>198</v>
@@ -5555,18 +5555,18 @@
         <v>189</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
       <c r="M56" s="11" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="N56" s="1"/>
       <c r="O56" s="1"/>
       <c r="P56" s="1"/>
       <c r="Q56" s="6" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="R56" s="1"/>
       <c r="S56" s="1"/>
@@ -5580,7 +5580,7 @@
         <v>38</v>
       </c>
       <c r="W56" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="Y56" t="s">
         <v>198</v>
@@ -5611,18 +5611,18 @@
         <v>189</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
       <c r="M57" s="11" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N57" s="1"/>
       <c r="O57" s="1"/>
       <c r="P57" s="1"/>
       <c r="Q57" s="6" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="R57" s="1"/>
       <c r="S57" s="1"/>
@@ -5636,7 +5636,7 @@
         <v>38</v>
       </c>
       <c r="W57" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="Y57" t="s">
         <v>198</v>
@@ -6118,7 +6118,7 @@
         <v>61</v>
       </c>
       <c r="X67" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="Y67" t="s">
         <v>198</v>
@@ -6173,7 +6173,7 @@
         <v>61</v>
       </c>
       <c r="X68" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="Y68" t="s">
         <v>198</v>
@@ -6228,7 +6228,7 @@
         <v>61</v>
       </c>
       <c r="X69" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="Y69" t="s">
         <v>198</v>
@@ -6259,7 +6259,7 @@
         <v>241</v>
       </c>
       <c r="J70" s="6" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="K70" s="1"/>
       <c r="L70" s="1"/>
@@ -6280,10 +6280,10 @@
         <v>205</v>
       </c>
       <c r="W70" s="14" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="X70" s="14" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="Y70" t="s">
         <v>198</v>
@@ -6314,7 +6314,7 @@
         <v>241</v>
       </c>
       <c r="J71" s="6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>
@@ -6335,7 +6335,7 @@
         <v>205</v>
       </c>
       <c r="W71" s="14" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="Y71" t="s">
         <v>198</v>
@@ -6366,7 +6366,7 @@
         <v>241</v>
       </c>
       <c r="J72" s="6" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="K72" s="1"/>
       <c r="L72" s="1"/>
@@ -6387,7 +6387,7 @@
         <v>205</v>
       </c>
       <c r="W72" s="14" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="Y72" t="s">
         <v>198</v>
@@ -6565,7 +6565,7 @@
       <c r="H76" s="1"/>
       <c r="I76" s="11"/>
       <c r="J76" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="K76" s="1"/>
       <c r="L76" s="1"/>
@@ -6586,10 +6586,10 @@
         <v>32</v>
       </c>
       <c r="W76" s="14" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="Y76" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="77" spans="1:25" ht="390" x14ac:dyDescent="0.25">
@@ -6615,7 +6615,7 @@
         <v>264</v>
       </c>
       <c r="J77" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="K77" s="1"/>
       <c r="L77" s="1"/>
@@ -6636,13 +6636,13 @@
         <v>205</v>
       </c>
       <c r="W77" s="14" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="X77" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="Y77" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="78" spans="1:25" ht="75" x14ac:dyDescent="0.25">
@@ -6670,7 +6670,7 @@
         <v>268</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="K78" s="1"/>
       <c r="L78" s="1"/>
@@ -6679,7 +6679,7 @@
       <c r="O78" s="1"/>
       <c r="P78" s="1"/>
       <c r="Q78" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="R78" s="1"/>
       <c r="S78" s="6"/>
@@ -6693,7 +6693,7 @@
         <v>205</v>
       </c>
       <c r="W78" s="14" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="Y78" t="s">
         <v>198</v>
@@ -6751,7 +6751,7 @@
         <v>61</v>
       </c>
       <c r="Y79" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="80" spans="1:25" ht="409.5" x14ac:dyDescent="0.25">
@@ -6779,7 +6779,7 @@
         <v>189</v>
       </c>
       <c r="J80" s="6" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="K80" s="1"/>
       <c r="L80" s="1"/>
@@ -6790,7 +6790,7 @@
       <c r="Q80" s="1"/>
       <c r="R80" s="1"/>
       <c r="S80" s="6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="T80" s="7" t="s">
         <v>24</v>
@@ -6802,7 +6802,7 @@
         <v>205</v>
       </c>
       <c r="W80" s="14" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="Y80" t="s">
         <v>198</v>
@@ -6833,18 +6833,18 @@
         <v>189</v>
       </c>
       <c r="J81" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="K81" s="1"/>
       <c r="L81" s="1"/>
       <c r="M81" s="15" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="N81" s="1"/>
       <c r="O81" s="1"/>
       <c r="P81" s="1"/>
       <c r="Q81" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="R81" s="1"/>
       <c r="S81" s="6"/>
@@ -6858,7 +6858,7 @@
         <v>205</v>
       </c>
       <c r="W81" s="14" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="82" spans="1:25" ht="409.5" x14ac:dyDescent="0.25">
@@ -6886,7 +6886,7 @@
         <v>189</v>
       </c>
       <c r="J82" s="6" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="K82" s="1"/>
       <c r="L82" s="1"/>
@@ -6897,7 +6897,7 @@
       <c r="Q82" s="1"/>
       <c r="R82" s="1"/>
       <c r="S82" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="T82" s="7" t="s">
         <v>24</v>
@@ -6909,7 +6909,7 @@
         <v>205</v>
       </c>
       <c r="W82" s="14" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="Y82" t="s">
         <v>198</v>

</xml_diff>

<commit_message>
correct harmo status detail for resting_heart_rate
</commit_message>
<xml_diff>
--- a/data_processing_elements-SHS.xlsx
+++ b/data_processing_elements-SHS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{100ECC84-4E17-4B36-964F-3F4494B42AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611EC3CC-BFEF-4592-836D-F1E9DEBD93BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
@@ -2366,10 +2366,10 @@
   <dimension ref="A1:AD84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="S17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="S14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W46" sqref="W46"/>
+      <selection pane="bottomRight" activeCell="V19" sqref="V19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="54.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3958,7 +3958,7 @@
         <v>50</v>
       </c>
       <c r="V27" t="s">
-        <v>32</v>
+        <v>205</v>
       </c>
       <c r="W27" s="14" t="s">
         <v>496</v>

</xml_diff>